<commit_message>
update gun_data.xlsx and develop_timetable.xlsx
</commit_message>
<xml_diff>
--- a/Data/develop_timetable.xlsx
+++ b/Data/develop_timetable.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13995" windowHeight="10440"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27870" windowHeight="12480"/>
   </bookViews>
   <sheets>
     <sheet name="what" sheetId="1" r:id="rId1"/>
@@ -19,16 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="102">
-  <si>
-    <t>枪名</t>
-  </si>
-  <si>
-    <t>建造时间</t>
-  </si>
-  <si>
-    <t>稀有度</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="105">
   <si>
     <t>柯尔特左轮</t>
   </si>
@@ -303,6 +294,9 @@
     <t>UMP9</t>
   </si>
   <si>
+    <t>UMP45</t>
+  </si>
+  <si>
     <t>OTs-12</t>
   </si>
   <si>
@@ -325,6 +319,21 @@
   </si>
   <si>
     <t>内格夫</t>
+  </si>
+  <si>
+    <t>谢尔久科夫</t>
+  </si>
+  <si>
+    <t>维尔德MkⅡ</t>
+  </si>
+  <si>
+    <t>索米</t>
+  </si>
+  <si>
+    <t>9A-91</t>
+  </si>
+  <si>
+    <t>Mk48</t>
   </si>
 </sst>
 </file>
@@ -1245,10 +1254,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C96"/>
+  <dimension ref="A1:C101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1258,354 +1267,354 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="B1" s="1">
+        <v>1.3888888888888888E-2</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1">
         <v>1.3888888888888888E-2</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1">
         <v>1.3888888888888888E-2</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1">
-        <v>1.3888888888888888E-2</v>
+        <v>1.5277777777777777E-2</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>80</v>
       </c>
       <c r="B5" s="1">
-        <v>1.5277777777777777E-2</v>
+        <v>1.7361111111111112E-2</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B6" s="1">
         <v>1.7361111111111112E-2</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>84</v>
+        <v>12</v>
       </c>
       <c r="B7" s="1">
-        <v>1.7361111111111112E-2</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B8" s="1">
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B9" s="1">
-        <v>2.0833333333333332E-2</v>
+        <v>2.4305555555555556E-2</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>100</v>
       </c>
       <c r="B10" s="1">
         <v>2.4305555555555556E-2</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B11" s="1">
         <v>2.7777777777777776E-2</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B12" s="1">
         <v>2.7777777777777776E-2</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B13" s="1">
         <v>2.7777777777777776E-2</v>
       </c>
       <c r="C13" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B14" s="1">
         <v>3.125E-2</v>
       </c>
       <c r="C14" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B15" s="1">
         <v>3.125E-2</v>
       </c>
       <c r="C15" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B16" s="1">
         <v>3.4722222222222224E-2</v>
       </c>
       <c r="C16" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B17" s="1">
         <v>3.4722222222222224E-2</v>
       </c>
       <c r="C17" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B18" s="1">
         <v>3.8194444444444441E-2</v>
       </c>
       <c r="C18" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B19" s="1">
         <v>3.8194444444444441E-2</v>
       </c>
       <c r="C19" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="B20" s="1">
-        <v>4.5138888888888888E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="C20" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>87</v>
       </c>
       <c r="B21" s="1">
-        <v>4.8611111111111112E-2</v>
+        <v>4.5138888888888888E-2</v>
       </c>
       <c r="C21" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>86</v>
+        <v>25</v>
       </c>
       <c r="B22" s="1">
         <v>4.8611111111111112E-2</v>
       </c>
       <c r="C22" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B23" s="1">
         <v>4.8611111111111112E-2</v>
       </c>
       <c r="C23" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>35</v>
+        <v>86</v>
       </c>
       <c r="B24" s="1">
-        <v>5.5555555555555552E-2</v>
+        <v>4.8611111111111112E-2</v>
       </c>
       <c r="C24" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>85</v>
+        <v>32</v>
       </c>
       <c r="B25" s="1">
         <v>5.5555555555555552E-2</v>
       </c>
       <c r="C25" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B26" s="1">
-        <v>5.9027777777777783E-2</v>
+        <v>5.5555555555555552E-2</v>
       </c>
       <c r="C26" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>22</v>
+        <v>84</v>
       </c>
       <c r="B27" s="1">
-        <v>6.25E-2</v>
+        <v>5.9027777777777783E-2</v>
       </c>
       <c r="C27" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B28" s="1">
         <v>6.25E-2</v>
       </c>
       <c r="C28" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B29" s="1">
         <v>6.25E-2</v>
       </c>
       <c r="C29" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B30" s="1">
-        <v>6.9444444444444434E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="C30" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B31" s="1">
         <v>6.9444444444444434E-2</v>
       </c>
       <c r="C31" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B32" s="1">
-        <v>7.6388888888888895E-2</v>
+        <v>6.9444444444444434E-2</v>
       </c>
       <c r="C32" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.15">
@@ -1613,527 +1622,527 @@
         <v>23</v>
       </c>
       <c r="B33" s="1">
-        <v>8.3333333333333329E-2</v>
+        <v>7.6388888888888895E-2</v>
       </c>
       <c r="C33" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B34" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="C34" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B35" s="1">
-        <v>9.0277777777777776E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="C35" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B36" s="1">
         <v>9.0277777777777776E-2</v>
       </c>
       <c r="C36" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
-        <v>93</v>
+        <v>24</v>
       </c>
       <c r="B37" s="1">
-        <v>9.375E-2</v>
+        <v>9.0277777777777776E-2</v>
       </c>
       <c r="C37" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="B38" s="1">
-        <v>9.7222222222222224E-2</v>
+        <v>9.375E-2</v>
       </c>
       <c r="C38" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
-        <v>20</v>
+        <v>91</v>
       </c>
       <c r="B39" s="1">
-        <v>0.10416666666666667</v>
+        <v>9.375E-2</v>
       </c>
       <c r="C39" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B40" s="1">
-        <v>0.1076388888888889</v>
+        <v>9.7222222222222224E-2</v>
       </c>
       <c r="C40" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
-        <v>67</v>
+        <v>102</v>
       </c>
       <c r="B41" s="1">
-        <v>0.1111111111111111</v>
+        <v>0.10069444444444443</v>
       </c>
       <c r="C41" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
-        <v>69</v>
+        <v>17</v>
       </c>
       <c r="B42" s="1">
-        <v>0.1111111111111111</v>
+        <v>0.10416666666666667</v>
       </c>
       <c r="C42" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
-        <v>96</v>
+        <v>22</v>
       </c>
       <c r="B43" s="1">
-        <v>0.11458333333333333</v>
+        <v>0.1076388888888889</v>
       </c>
       <c r="C43" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B44" s="1">
-        <v>0.11805555555555557</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="C44" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B45" s="1">
-        <v>0.11805555555555557</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="C45" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
-        <v>58</v>
+        <v>94</v>
       </c>
       <c r="B46" s="1">
-        <v>0.125</v>
+        <v>0.11458333333333333</v>
       </c>
       <c r="C46" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="B47" s="1">
-        <v>0.13194444444444445</v>
+        <v>0.11805555555555557</v>
       </c>
       <c r="C47" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="B48" s="1">
-        <v>0.13194444444444445</v>
+        <v>0.11805555555555557</v>
       </c>
       <c r="C48" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
-        <v>94</v>
+        <v>55</v>
       </c>
       <c r="B49" s="1">
-        <v>0.13194444444444445</v>
+        <v>0.125</v>
       </c>
       <c r="C49" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
-        <v>97</v>
+        <v>43</v>
       </c>
       <c r="B50" s="1">
         <v>0.13194444444444445</v>
       </c>
       <c r="C50" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A51" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B51" s="1">
-        <v>0.1388888888888889</v>
+        <v>0.13194444444444445</v>
       </c>
       <c r="C51" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A52" t="s">
-        <v>56</v>
+        <v>92</v>
       </c>
       <c r="B52" s="1">
-        <v>0.1388888888888889</v>
+        <v>0.13194444444444445</v>
       </c>
       <c r="C52" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A53" t="s">
-        <v>66</v>
+        <v>95</v>
       </c>
       <c r="B53" s="1">
-        <v>0.1388888888888889</v>
+        <v>0.13194444444444445</v>
       </c>
       <c r="C53" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A54" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="B54" s="1">
-        <v>0.1423611111111111</v>
+        <v>0.1388888888888889</v>
       </c>
       <c r="C54" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A55" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="B55" s="1">
-        <v>0.14583333333333334</v>
+        <v>0.1388888888888889</v>
       </c>
       <c r="C55" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A56" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="B56" s="1">
-        <v>0.14583333333333334</v>
+        <v>0.1388888888888889</v>
       </c>
       <c r="C56" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A57" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B57" s="1">
-        <v>0.14583333333333334</v>
+        <v>0.1423611111111111</v>
       </c>
       <c r="C57" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A58" t="s">
-        <v>65</v>
+        <v>38</v>
       </c>
       <c r="B58" s="1">
         <v>0.14583333333333334</v>
       </c>
       <c r="C58" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A59" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
       <c r="B59" s="1">
         <v>0.14583333333333334</v>
       </c>
       <c r="C59" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A60" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B60" s="1">
-        <v>0.14930555555555555</v>
+        <v>0.14583333333333334</v>
       </c>
       <c r="C60" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A61" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="B61" s="1">
-        <v>0.14930555555555555</v>
+        <v>0.14583333333333334</v>
       </c>
       <c r="C61" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A62" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="B62" s="1">
-        <v>0.14930555555555555</v>
+        <v>0.14583333333333334</v>
       </c>
       <c r="C62" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A63" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B63" s="1">
         <v>0.14930555555555555</v>
       </c>
       <c r="C63" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A64" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="B64" s="1">
-        <v>0.15277777777777776</v>
+        <v>0.14930555555555555</v>
       </c>
       <c r="C64" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A65" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B65" s="1">
-        <v>0.15277777777777776</v>
+        <v>0.14930555555555555</v>
       </c>
       <c r="C65" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A66" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B66" s="1">
-        <v>0.15277777777777776</v>
+        <v>0.14930555555555555</v>
       </c>
       <c r="C66" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A67" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="B67" s="1">
-        <v>0.15625</v>
+        <v>0.14930555555555555</v>
       </c>
       <c r="C67" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A68" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B68" s="1">
-        <v>0.15972222222222224</v>
+        <v>0.15277777777777776</v>
       </c>
       <c r="C68" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A69" t="s">
-        <v>88</v>
+        <v>41</v>
       </c>
       <c r="B69" s="1">
-        <v>0.15972222222222224</v>
+        <v>0.15277777777777776</v>
       </c>
       <c r="C69" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A70" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B70" s="1">
-        <v>0.16319444444444445</v>
+        <v>0.15277777777777776</v>
       </c>
       <c r="C70" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A71" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="B71" s="1">
-        <v>0.16666666666666666</v>
+        <v>0.15625</v>
       </c>
       <c r="C71" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A72" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="B72" s="1">
-        <v>0.17013888888888887</v>
+        <v>0.15972222222222224</v>
       </c>
       <c r="C72" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A73" t="s">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="B73" s="1">
-        <v>0.17361111111111113</v>
+        <v>0.15972222222222224</v>
       </c>
       <c r="C73" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A74" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="B74" s="1">
-        <v>0.18402777777777779</v>
+        <v>0.16319444444444445</v>
       </c>
       <c r="C74" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A75" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B75" s="1">
-        <v>0.1875</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="C75" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A76" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="B76" s="1">
-        <v>0.19444444444444445</v>
+        <v>0.17013888888888887</v>
       </c>
       <c r="C76" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A77" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B77" s="1">
-        <v>0.19791666666666666</v>
+        <v>0.17361111111111113</v>
       </c>
       <c r="C77" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A78" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="B78" s="1">
-        <v>0.20138888888888887</v>
+        <v>0.18402777777777779</v>
       </c>
       <c r="C78" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A79" t="s">
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="B79" s="1">
-        <v>0.20138888888888887</v>
+        <v>0.1875</v>
       </c>
       <c r="C79" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A80" t="s">
-        <v>100</v>
+        <v>42</v>
       </c>
       <c r="B80" s="1">
-        <v>0.20138888888888887</v>
+        <v>0.19444444444444445</v>
       </c>
       <c r="C80" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.15">
@@ -2141,54 +2150,54 @@
         <v>48</v>
       </c>
       <c r="B81" s="1">
-        <v>0.20833333333333334</v>
+        <v>0.19791666666666666</v>
       </c>
       <c r="C81" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A82" t="s">
-        <v>76</v>
+        <v>44</v>
       </c>
       <c r="B82" s="1">
-        <v>0.20833333333333334</v>
+        <v>0.20138888888888887</v>
       </c>
       <c r="C82" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A83" t="s">
-        <v>80</v>
+        <v>97</v>
       </c>
       <c r="B83" s="1">
-        <v>0.20833333333333334</v>
+        <v>0.20138888888888887</v>
       </c>
       <c r="C83" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A84" t="s">
-        <v>75</v>
+        <v>98</v>
       </c>
       <c r="B84" s="1">
-        <v>0.21527777777777779</v>
+        <v>0.20138888888888887</v>
       </c>
       <c r="C84" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A85" t="s">
-        <v>82</v>
+        <v>45</v>
       </c>
       <c r="B85" s="1">
-        <v>0.22222222222222221</v>
+        <v>0.20833333333333334</v>
       </c>
       <c r="C85" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.15">
@@ -2196,10 +2205,10 @@
         <v>73</v>
       </c>
       <c r="B86" s="1">
-        <v>0.22916666666666666</v>
+        <v>0.20833333333333334</v>
       </c>
       <c r="C86" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.15">
@@ -2207,21 +2216,21 @@
         <v>77</v>
       </c>
       <c r="B87" s="1">
-        <v>0.22916666666666666</v>
+        <v>0.20833333333333334</v>
       </c>
       <c r="C87" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A88" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B88" s="1">
-        <v>0.23611111111111113</v>
+        <v>0.21527777777777779</v>
       </c>
       <c r="C88" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.15">
@@ -2229,94 +2238,150 @@
         <v>79</v>
       </c>
       <c r="B89" s="1">
-        <v>0.24305555555555555</v>
+        <v>0.22222222222222221</v>
       </c>
       <c r="C89" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A90" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B90" s="1">
-        <v>0.25694444444444448</v>
+        <v>0.22916666666666666</v>
       </c>
       <c r="C90" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A91" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B91" s="1">
-        <v>0.25694444444444448</v>
+        <v>0.22916666666666666</v>
       </c>
       <c r="C91" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A92" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B92" s="1">
-        <v>0.2673611111111111</v>
+        <v>0.23611111111111113</v>
       </c>
       <c r="C92" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A93" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B93" s="1">
-        <v>0.27083333333333331</v>
+        <v>0.24305555555555555</v>
       </c>
       <c r="C93" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A94" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="B94" s="1">
-        <v>0.27083333333333331</v>
+        <v>0.25694444444444448</v>
       </c>
       <c r="C94" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A95" t="s">
-        <v>101</v>
+        <v>69</v>
       </c>
       <c r="B95" s="1">
-        <v>0.27430555555555552</v>
+        <v>0.25694444444444448</v>
       </c>
       <c r="C95" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A96" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="B96" s="1">
+        <v>0.2638888888888889</v>
+      </c>
+      <c r="C96" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A97" t="s">
+        <v>67</v>
+      </c>
+      <c r="B97" s="1">
+        <v>0.2673611111111111</v>
+      </c>
+      <c r="C97" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A98" t="s">
+        <v>75</v>
+      </c>
+      <c r="B98" s="1">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="C98" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A99" t="s">
+        <v>78</v>
+      </c>
+      <c r="B99" s="1">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="C99" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A100" t="s">
+        <v>99</v>
+      </c>
+      <c r="B100" s="1">
+        <v>0.27430555555555552</v>
+      </c>
+      <c r="C100" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A101" t="s">
+        <v>96</v>
+      </c>
+      <c r="B101" s="1">
         <v>0.28125</v>
       </c>
-      <c r="C96" t="s">
-        <v>21</v>
+      <c r="C101" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:C96">
-    <sortCondition ref="B19"/>
+  <sortState ref="A1:C101">
+    <sortCondition ref="B1"/>
   </sortState>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>